<commit_message>
Updated prototype costs after ordering most parts, still lacking rotary encoder knobs, and minor updates to PCB that didn't get committed before
</commit_message>
<xml_diff>
--- a/Prototype_cost.xlsx
+++ b/Prototype_cost.xlsx
@@ -8,24 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seth\Documents\KiCad\Rocketboard-16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D386D124-FD58-4A08-A37F-67454325EB77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DF274E-CA73-4E15-847D-AEC4EC0FDFE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Vender</t>
   </si>
@@ -39,12 +47,6 @@
     <t>Aliexpress</t>
   </si>
   <si>
-    <t>SK6812Mini-E RGB LEDs x 100</t>
-  </si>
-  <si>
-    <t>Mill-Max 0305-2-15-80-47-80-10 x 200</t>
-  </si>
-  <si>
     <t>u/tonsoffun</t>
   </si>
   <si>
@@ -60,7 +62,79 @@
     <t>Parts (see LCSC BOM)</t>
   </si>
   <si>
-    <t>SSD1306 128x64 OLED Display x 5</t>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Not able to find these anywhere else, shipping is slow Aliexpress value shipping</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SK6812Mini-E RGB LEDs </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x 100</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mill-Max 0305-2-15-80-47-80-10 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x 200</t>
+    </r>
+  </si>
+  <si>
+    <t>Cheaper than Mouser order, $18 + $7 shipping</t>
+  </si>
+  <si>
+    <t>Saved $15 on shipping with a first order coupon</t>
+  </si>
+  <si>
+    <t>Went with FedEx International for about $10 less shipping</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <r>
+      <t>SSD1306 128x64 OLED Display</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> x 6</t>
+    </r>
+  </si>
+  <si>
+    <t>Bought 4 blue PCBs and 2 black PCBs, both white pixels</t>
+  </si>
+  <si>
+    <t>Rotary encoder knobs</t>
   </si>
 </sst>
 </file>
@@ -69,9 +143,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +154,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -108,9 +190,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -392,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -403,9 +488,10 @@
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="65.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -415,51 +501,96 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
         <v>11.28</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>34.909999999999997</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C5" s="1">
+        <v>59.85</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="C6" s="1">
+        <v>33.32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1">
+        <f>SUM(C2:C7)</f>
+        <v>164.35999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>